<commit_message>
CSV: make sure all lines in csv have the same number of columns
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF7BFEF-A195-412A-AAC3-834FE76F616B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FA7698-E6D8-48F8-B0D5-575791552865}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5160" yWindow="5100" windowWidth="21600" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -412,21 +412,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>